<commit_message>
/ ‘Revised Communities_Plan functionality list_V6.xlsx’
</commit_message>
<xml_diff>
--- a/Revised Communities_Plan functionality list_V6.xlsx
+++ b/Revised Communities_Plan functionality list_V6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33660" yWindow="-2640" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Home Page</t>
   </si>
@@ -119,10 +119,6 @@
   </si>
   <si>
     <t>CSAT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Profanity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -134,12 +130,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -553,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:A38"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -688,91 +678,84 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="2"/>
+      <c r="A24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="9">
+        <v>41220</v>
+      </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="9">
-        <v>41220</v>
-      </c>
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="2"/>
+      <c r="A27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="9">
+        <v>41241</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="9">
-        <v>41241</v>
-      </c>
+      <c r="A28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1">
-      <c r="A32" s="4" t="s">
+    <row r="31" spans="1:2" ht="15" thickBot="1">
+      <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B31" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>